<commit_message>
Updated Logistics DocTypes; TICC-411
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.4.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/dev/git-peppol/edec-codelists/work-in-progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4F1651-CBA5-B44F-981E-2871674E2FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23917F2D-71A3-434A-BBFF-8C369786D4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="23980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="1040" windowWidth="38860" windowHeight="23680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2704" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="860">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2672,6 +2672,34 @@
   </si>
   <si>
     <t>Peppol Receipt Advice V1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:fdc:peppol.eu:logistics:trns:application_response:1::2.1</t>
+  </si>
+  <si>
+    <t>TICC-411</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:logistics:bis:advanced_transport_execution_plan:1</t>
+  </si>
+  <si>
+    <t>Peppol Logistics Application Response V1</t>
+  </si>
+  <si>
+    <t>Peppol Transport Execution Plan Request V1.2</t>
+  </si>
+  <si>
+    <t>Peppol Transport Execution Plan V1.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:TransportExecutionPlanRequest-2::TransportExecutionPlanRequest##urn:fdc:peppol.eu:logistics:trns:transport_execution_plan_request:1::2.4</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:TransportExecutionPlan-2::TransportExecutionPlan##urn:fdc:peppol.eu:logistics:trns:transport_execution_plan:1::2.4</t>
+  </si>
+  <si>
+    <t>TICC-267
+TICC-411</t>
   </si>
 </sst>
 </file>
@@ -2798,7 +2826,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2925,6 +2953,7 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3338,11 +3367,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N307"/>
+  <dimension ref="A1:N310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A195" sqref="A195"/>
+      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A311" sqref="A311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11483,79 +11512,91 @@
         <v>546</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A214" s="5" t="s">
+    <row r="214" spans="1:14" s="31" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A214" s="31" t="s">
         <v>845</v>
       </c>
-      <c r="B214" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C214" s="5" t="s">
+      <c r="B214" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C214" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="D214" s="23" t="s">
+      <c r="D214" s="28" t="s">
         <v>556</v>
       </c>
-      <c r="E214" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="H214" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="I214" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J214" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K214" s="20">
-        <v>1</v>
-      </c>
-      <c r="L214" s="4" t="s">
+      <c r="E214" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="F214" s="35" t="s">
+        <v>839</v>
+      </c>
+      <c r="G214" s="42">
+        <v>46025</v>
+      </c>
+      <c r="H214" s="31" t="s">
+        <v>859</v>
+      </c>
+      <c r="I214" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J214" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K214" s="29">
+        <v>1</v>
+      </c>
+      <c r="L214" s="27" t="s">
         <v>841</v>
       </c>
-      <c r="M214" s="4" t="s">
+      <c r="M214" s="27" t="s">
         <v>841</v>
       </c>
-      <c r="N214" s="36" t="s">
+      <c r="N214" s="46" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A215" s="5" t="s">
+    <row r="215" spans="1:14" s="31" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A215" s="31" t="s">
         <v>846</v>
       </c>
-      <c r="B215" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C215" s="5" t="s">
+      <c r="B215" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C215" s="31" t="s">
         <v>558</v>
       </c>
-      <c r="D215" s="23" t="s">
+      <c r="D215" s="28" t="s">
         <v>556</v>
       </c>
-      <c r="E215" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="H215" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="I215" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J215" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K215" s="20">
-        <v>1</v>
-      </c>
-      <c r="L215" s="4" t="s">
+      <c r="E215" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="F215" s="35" t="s">
+        <v>839</v>
+      </c>
+      <c r="G215" s="42">
+        <v>46025</v>
+      </c>
+      <c r="H215" s="31" t="s">
+        <v>859</v>
+      </c>
+      <c r="I215" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J215" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K215" s="29">
+        <v>1</v>
+      </c>
+      <c r="L215" s="27" t="s">
         <v>841</v>
       </c>
-      <c r="M215" s="4" t="s">
+      <c r="M215" s="27" t="s">
         <v>841</v>
       </c>
-      <c r="N215" s="36" t="s">
+      <c r="N215" s="46" t="s">
         <v>550</v>
       </c>
     </row>
@@ -15008,6 +15049,121 @@
       </c>
       <c r="N307" s="5" t="s">
         <v>578</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>854</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C308" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="D308" s="24" t="s">
+        <v>839</v>
+      </c>
+      <c r="E308" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="H308" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="I308" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J308" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K308" s="20">
+        <v>1</v>
+      </c>
+      <c r="L308" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="M308" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="N308" s="5" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A309" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="B309" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C309" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="D309" s="24" t="s">
+        <v>839</v>
+      </c>
+      <c r="E309" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="H309" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="I309" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J309" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K309" s="20">
+        <v>1</v>
+      </c>
+      <c r="L309" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="M309" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="N309" s="36" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A310" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="B310" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C310" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="D310" s="24" t="s">
+        <v>839</v>
+      </c>
+      <c r="E310" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="H310" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="I310" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J310" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K310" s="20">
+        <v>1</v>
+      </c>
+      <c r="L310" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="M310" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="N310" s="36" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>